<commit_message>
Handle renamed field in TP spreadsheets
TP renamed a field in the spreadsheet they provide for call data, these
changes ensure we retrieve the call date correctly.
</commit_message>
<xml_diff>
--- a/spec/fixtures/TP-20160505.xlsx
+++ b/spec/fixtures/TP-20160505.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
-    <t>Call Date</t>
+    <t>FormatDate</t>
   </si>
   <si>
     <t>Team+</t>
@@ -105,7 +105,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m&quot;/&quot;d&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -117,19 +117,15 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Arial"/>
+      <name val="Verdana"/>
     </font>
     <font>
-      <sz val="13"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
+      <b val="1"/>
       <sz val="9"/>
       <color indexed="9"/>
-      <name val="Arial Bold"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="9"/>
@@ -163,7 +159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -201,39 +197,159 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top style="thin">
+        <color indexed="12"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="15"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="15"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="15"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="59" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="right" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment horizontal="left" vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="5" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="59" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="right" vertical="bottom"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -258,6 +374,7 @@
       <rgbColor rgb="ffebebeb"/>
       <rgbColor rgb="ff333333"/>
       <rgbColor rgb="fff8fbfc"/>
+      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -274,10 +391,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="404040"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="BFBFBF"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -316,53 +433,8 @@
         <a:cs typeface="Helvetica"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Blank">
       <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="100000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="129999"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:shade val="100000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -431,27 +503,6 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="104999"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
         <a:effectStyle>
@@ -477,33 +528,6 @@
             <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
               <a:srgbClr val="000000">
                 <a:alpha val="50000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -558,68 +582,21 @@
             <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
           </a:path>
         </a:gradFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:blipFill rotWithShape="1">
-          <a:blip r:embed="rId1"/>
-          <a:srcRect l="0" t="0" r="0" b="0"/>
-          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
-        </a:blipFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:solidFill>
+          <a:srgbClr val="FFFFFF"/>
+        </a:solidFill>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -628,40 +605,35 @@
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst>
-              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
-                <a:srgbClr val="000000">
-                  <a:alpha val="31034"/>
-                </a:srgbClr>
-              </a:outerShdw>
-            </a:effectLst>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -914,14 +886,21 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="6350" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
-        <a:effectLst/>
+        <a:effectLst>
+          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
+            <a:srgbClr val="000000">
+              <a:alpha val="50000"/>
+            </a:srgbClr>
+          </a:outerShdw>
+        </a:effectLst>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -1203,12 +1182,13 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
+        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1486,7 +1466,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N4"/>
+  <dimension ref="A1:N10"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1581,51 +1561,51 @@
       <c r="I2" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="J2" s="4"/>
-      <c r="K2" s="4"/>
-      <c r="L2" s="4"/>
+      <c r="J2" s="6"/>
+      <c r="K2" s="6"/>
+      <c r="L2" s="6"/>
       <c r="M2" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="N2" s="4"/>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" ht="19.7" customHeight="1">
-      <c r="A3" s="6">
+      <c r="A3" s="7">
         <v>42494</v>
       </c>
-      <c r="B3" t="s" s="7">
+      <c r="B3" t="s" s="8">
         <v>14</v>
       </c>
-      <c r="C3" t="s" s="7">
+      <c r="C3" t="s" s="8">
         <v>19</v>
       </c>
-      <c r="D3" t="s" s="7">
+      <c r="D3" t="s" s="8">
         <v>20</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="9">
         <v>150.238006591797</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="9">
         <v>0</v>
       </c>
-      <c r="G3" s="8">
+      <c r="G3" s="9">
         <v>150.100997924805</v>
       </c>
-      <c r="H3" s="8">
+      <c r="H3" s="9">
         <v>0.221000000834465</v>
       </c>
-      <c r="I3" t="s" s="7">
+      <c r="I3" t="s" s="8">
         <v>21</v>
       </c>
-      <c r="J3" s="7"/>
-      <c r="K3" t="s" s="7">
+      <c r="J3" s="10"/>
+      <c r="K3" t="s" s="8">
         <v>22</v>
       </c>
-      <c r="L3" s="7"/>
-      <c r="M3" t="s" s="7">
+      <c r="L3" s="10"/>
+      <c r="M3" t="s" s="8">
         <v>23</v>
       </c>
-      <c r="N3" s="7"/>
+      <c r="N3" s="10"/>
     </row>
     <row r="4" ht="19.7" customHeight="1">
       <c r="A4" s="3">
@@ -1655,15 +1635,111 @@
       <c r="I4" t="s" s="4">
         <v>26</v>
       </c>
-      <c r="J4" s="4"/>
+      <c r="J4" s="6"/>
       <c r="K4" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="L4" s="4"/>
+      <c r="L4" s="6"/>
       <c r="M4" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="N4" s="4"/>
+      <c r="N4" s="6"/>
+    </row>
+    <row r="5" ht="18" customHeight="1">
+      <c r="A5" s="11"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="12"/>
+      <c r="D5" s="12"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="12"/>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+      <c r="J5" s="12"/>
+      <c r="K5" s="12"/>
+      <c r="L5" s="12"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="13"/>
+    </row>
+    <row r="6" ht="18" customHeight="1">
+      <c r="A6" s="14"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="16"/>
+    </row>
+    <row r="7" ht="18" customHeight="1">
+      <c r="A7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="15"/>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="16"/>
+    </row>
+    <row r="8" ht="18" customHeight="1">
+      <c r="A8" s="14"/>
+      <c r="B8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="15"/>
+      <c r="E8" s="15"/>
+      <c r="F8" s="15"/>
+      <c r="G8" s="15"/>
+      <c r="H8" s="15"/>
+      <c r="I8" s="15"/>
+      <c r="J8" s="15"/>
+      <c r="K8" s="15"/>
+      <c r="L8" s="15"/>
+      <c r="M8" s="15"/>
+      <c r="N8" s="16"/>
+    </row>
+    <row r="9" ht="18" customHeight="1">
+      <c r="A9" s="14"/>
+      <c r="B9" s="15"/>
+      <c r="C9" s="15"/>
+      <c r="D9" s="15"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="15"/>
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="15"/>
+      <c r="M9" s="15"/>
+      <c r="N9" s="16"/>
+    </row>
+    <row r="10" ht="18" customHeight="1">
+      <c r="A10" s="17"/>
+      <c r="B10" s="18"/>
+      <c r="C10" s="18"/>
+      <c r="D10" s="18"/>
+      <c r="E10" s="18"/>
+      <c r="F10" s="18"/>
+      <c r="G10" s="18"/>
+      <c r="H10" s="18"/>
+      <c r="I10" s="18"/>
+      <c r="J10" s="18"/>
+      <c r="K10" s="18"/>
+      <c r="L10" s="18"/>
+      <c r="M10" s="18"/>
+      <c r="N10" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>

<commit_message>
Revert "Handle renamed field in TP spreadsheets"
</commit_message>
<xml_diff>
--- a/spec/fixtures/TP-20160505.xlsx
+++ b/spec/fixtures/TP-20160505.xlsx
@@ -13,7 +13,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="28">
   <si>
-    <t>FormatDate</t>
+    <t>Call Date</t>
   </si>
   <si>
     <t>Team+</t>
@@ -105,7 +105,7 @@
     <numFmt numFmtId="0" formatCode="General"/>
     <numFmt numFmtId="59" formatCode="m&quot;/&quot;d&quot;/&quot;yyyy"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="12"/>
       <color indexed="8"/>
@@ -117,15 +117,19 @@
       <name val="Helvetica"/>
     </font>
     <font>
-      <sz val="15"/>
+      <sz val="10"/>
       <color indexed="8"/>
-      <name val="Verdana"/>
+      <name val="Arial"/>
     </font>
     <font>
-      <b val="1"/>
+      <sz val="13"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+    </font>
+    <font>
       <sz val="9"/>
       <color indexed="9"/>
-      <name val="Arial"/>
+      <name val="Arial Bold"/>
     </font>
     <font>
       <sz val="9"/>
@@ -159,7 +163,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -197,159 +201,39 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top style="thin">
-        <color indexed="12"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="15"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="15"/>
-      </right>
-      <top/>
-      <bottom style="thin">
-        <color indexed="15"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+      <alignment vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="5" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="1" fontId="4" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="59" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="59" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="left" vertical="bottom"/>
     </xf>
-    <xf numFmtId="49" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="1" fontId="4" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="1" fontId="5" fillId="4" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="right" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="left" vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="9" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="10" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="11" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="bottom"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -374,7 +258,6 @@
       <rgbColor rgb="ffebebeb"/>
       <rgbColor rgb="ff333333"/>
       <rgbColor rgb="fff8fbfc"/>
-      <rgbColor rgb="ffaaaaaa"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -391,10 +274,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="A7A7A7"/>
+        <a:srgbClr val="404040"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="535353"/>
+        <a:srgbClr val="BFBFBF"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="499BC9"/>
@@ -433,7 +316,7 @@
         <a:cs typeface="Helvetica"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Blank">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -480,8 +363,74 @@
           </a:gsLst>
           <a:lin ang="16200000" scaled="0"/>
         </a:gradFill>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="100000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="129999"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:shade val="100000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="104999"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
         <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
@@ -532,8 +481,83 @@
             </a:outerShdw>
           </a:effectLst>
         </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="20000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="40000" dist="23000" dir="5400000">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
       </a:effectStyleLst>
       <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -588,15 +612,14 @@
   <a:objectDefaults>
     <a:spDef>
       <a:spPr>
-        <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
-        </a:solidFill>
-        <a:ln w="25400" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
+        <a:blipFill rotWithShape="1">
+          <a:blip r:embed="rId1"/>
+          <a:srcRect l="0" t="0" r="0" b="0"/>
+          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
+        </a:blipFill>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst>
           <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
@@ -605,35 +628,40 @@
             </a:srgbClr>
           </a:outerShdw>
         </a:effectLst>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="ctr" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:tabLst/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:tabLst/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:effectLst>
+              <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="25400" dist="23998" dir="2700000">
+                <a:srgbClr val="000000">
+                  <a:alpha val="31034"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
             <a:uFillTx/>
             <a:latin typeface="+mn-lt"/>
             <a:ea typeface="+mn-ea"/>
@@ -886,21 +914,14 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="6350" cap="flat">
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="400000"/>
         </a:ln>
-        <a:effectLst>
-          <a:outerShdw sx="100000" sy="100000" kx="0" ky="0" algn="b" rotWithShape="0" blurRad="38100" dist="25400" dir="5400000">
-            <a:srgbClr val="000000">
-              <a:alpha val="50000"/>
-            </a:srgbClr>
-          </a:outerShdw>
-        </a:effectLst>
-        <a:sp3d/>
+        <a:effectLst/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="91439" tIns="45719" rIns="91439" bIns="45719" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:noAutofit/>
@@ -1182,13 +1203,12 @@
           <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
-        <a:sp3d/>
       </a:spPr>
       <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="overflow" horzOverflow="overflow" vert="horz" wrap="square" lIns="50800" tIns="50800" rIns="50800" bIns="50800" numCol="1" spcCol="38100" rtlCol="0" anchor="t" upright="0">
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1466,7 +1486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:N10"/>
+  <dimension ref="A1:N4"/>
   <sheetViews>
     <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
@@ -1561,51 +1581,51 @@
       <c r="I2" t="s" s="4">
         <v>17</v>
       </c>
-      <c r="J2" s="6"/>
-      <c r="K2" s="6"/>
-      <c r="L2" s="6"/>
+      <c r="J2" s="4"/>
+      <c r="K2" s="4"/>
+      <c r="L2" s="4"/>
       <c r="M2" t="s" s="4">
         <v>18</v>
       </c>
-      <c r="N2" s="6"/>
+      <c r="N2" s="4"/>
     </row>
     <row r="3" ht="19.7" customHeight="1">
-      <c r="A3" s="7">
+      <c r="A3" s="6">
         <v>42494</v>
       </c>
-      <c r="B3" t="s" s="8">
+      <c r="B3" t="s" s="7">
         <v>14</v>
       </c>
-      <c r="C3" t="s" s="8">
+      <c r="C3" t="s" s="7">
         <v>19</v>
       </c>
-      <c r="D3" t="s" s="8">
+      <c r="D3" t="s" s="7">
         <v>20</v>
       </c>
-      <c r="E3" s="9">
+      <c r="E3" s="8">
         <v>150.238006591797</v>
       </c>
-      <c r="F3" s="9">
+      <c r="F3" s="8">
         <v>0</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="8">
         <v>150.100997924805</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="8">
         <v>0.221000000834465</v>
       </c>
-      <c r="I3" t="s" s="8">
+      <c r="I3" t="s" s="7">
         <v>21</v>
       </c>
-      <c r="J3" s="10"/>
-      <c r="K3" t="s" s="8">
+      <c r="J3" s="7"/>
+      <c r="K3" t="s" s="7">
         <v>22</v>
       </c>
-      <c r="L3" s="10"/>
-      <c r="M3" t="s" s="8">
+      <c r="L3" s="7"/>
+      <c r="M3" t="s" s="7">
         <v>23</v>
       </c>
-      <c r="N3" s="10"/>
+      <c r="N3" s="7"/>
     </row>
     <row r="4" ht="19.7" customHeight="1">
       <c r="A4" s="3">
@@ -1635,111 +1655,15 @@
       <c r="I4" t="s" s="4">
         <v>26</v>
       </c>
-      <c r="J4" s="6"/>
+      <c r="J4" s="4"/>
       <c r="K4" t="s" s="4">
         <v>27</v>
       </c>
-      <c r="L4" s="6"/>
+      <c r="L4" s="4"/>
       <c r="M4" t="s" s="4">
         <v>23</v>
       </c>
-      <c r="N4" s="6"/>
-    </row>
-    <row r="5" ht="18" customHeight="1">
-      <c r="A5" s="11"/>
-      <c r="B5" s="12"/>
-      <c r="C5" s="12"/>
-      <c r="D5" s="12"/>
-      <c r="E5" s="12"/>
-      <c r="F5" s="12"/>
-      <c r="G5" s="12"/>
-      <c r="H5" s="12"/>
-      <c r="I5" s="12"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="12"/>
-      <c r="L5" s="12"/>
-      <c r="M5" s="12"/>
-      <c r="N5" s="13"/>
-    </row>
-    <row r="6" ht="18" customHeight="1">
-      <c r="A6" s="14"/>
-      <c r="B6" s="15"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15"/>
-      <c r="F6" s="15"/>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="M6" s="15"/>
-      <c r="N6" s="16"/>
-    </row>
-    <row r="7" ht="18" customHeight="1">
-      <c r="A7" s="14"/>
-      <c r="B7" s="15"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15"/>
-      <c r="F7" s="15"/>
-      <c r="G7" s="15"/>
-      <c r="H7" s="15"/>
-      <c r="I7" s="15"/>
-      <c r="J7" s="15"/>
-      <c r="K7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="M7" s="15"/>
-      <c r="N7" s="16"/>
-    </row>
-    <row r="8" ht="18" customHeight="1">
-      <c r="A8" s="14"/>
-      <c r="B8" s="15"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="15"/>
-      <c r="E8" s="15"/>
-      <c r="F8" s="15"/>
-      <c r="G8" s="15"/>
-      <c r="H8" s="15"/>
-      <c r="I8" s="15"/>
-      <c r="J8" s="15"/>
-      <c r="K8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="M8" s="15"/>
-      <c r="N8" s="16"/>
-    </row>
-    <row r="9" ht="18" customHeight="1">
-      <c r="A9" s="14"/>
-      <c r="B9" s="15"/>
-      <c r="C9" s="15"/>
-      <c r="D9" s="15"/>
-      <c r="E9" s="15"/>
-      <c r="F9" s="15"/>
-      <c r="G9" s="15"/>
-      <c r="H9" s="15"/>
-      <c r="I9" s="15"/>
-      <c r="J9" s="15"/>
-      <c r="K9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="15"/>
-      <c r="N9" s="16"/>
-    </row>
-    <row r="10" ht="18" customHeight="1">
-      <c r="A10" s="17"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="18"/>
-      <c r="D10" s="18"/>
-      <c r="E10" s="18"/>
-      <c r="F10" s="18"/>
-      <c r="G10" s="18"/>
-      <c r="H10" s="18"/>
-      <c r="I10" s="18"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="18"/>
-      <c r="N10" s="19"/>
+      <c r="N4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>